<commit_message>
Performance results obtained for all java benchmarks in renaissance.
</commit_message>
<xml_diff>
--- a/evaluation/performance/results/actors.xlsx
+++ b/evaluation/performance/results/actors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\evaluation\performance\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D698DF-3895-4BA8-904B-CD1A5349E6F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6A2621-2540-4ED2-BA85-DB6FB6D7B9E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,19 @@
     <sheet name="akka-uct" sheetId="1" r:id="rId1"/>
     <sheet name="reactors" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -58,7 +67,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,6 +78,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -95,10 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,195 +423,207 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>34453906954</v>
-      </c>
-      <c r="B2" s="1">
-        <v>29501633186</v>
+      <c r="A2" s="2">
+        <v>29674499277</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20115916962</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>29674499277</v>
-      </c>
-      <c r="B3" s="2">
-        <v>20115916962</v>
+      <c r="A3" s="1">
+        <v>33498155364</v>
+      </c>
+      <c r="B3" s="1">
+        <v>19608649637</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>33498155364</v>
-      </c>
-      <c r="B4" s="1">
-        <v>19608649637</v>
+      <c r="A4" s="2">
+        <v>40973070240</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20726383531</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>40973070240</v>
-      </c>
-      <c r="B5" s="2">
-        <v>20726383531</v>
+      <c r="A5" s="1">
+        <v>42583330030</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20007287213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42583330030</v>
-      </c>
-      <c r="B6" s="1">
-        <v>20007287213</v>
+      <c r="A6" s="2">
+        <v>44018474553</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20330624273</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>44018474553</v>
-      </c>
-      <c r="B7" s="2">
-        <v>20330624273</v>
+      <c r="A7" s="1">
+        <v>43626981341</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20228668474</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>43626981341</v>
-      </c>
-      <c r="B8" s="1">
-        <v>20228668474</v>
+      <c r="A8" s="2">
+        <v>46081101502</v>
+      </c>
+      <c r="B8" s="2">
+        <v>23409417374</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>46081101502</v>
-      </c>
-      <c r="B9" s="2">
-        <v>23409417374</v>
+      <c r="A9" s="1">
+        <v>47489388724</v>
+      </c>
+      <c r="B9" s="1">
+        <v>26208756959</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>47489388724</v>
-      </c>
-      <c r="B10" s="1">
-        <v>26208756959</v>
+      <c r="A10" s="2">
+        <v>47752814705</v>
+      </c>
+      <c r="B10" s="2">
+        <v>27416014289</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>47752814705</v>
-      </c>
-      <c r="B11" s="2">
-        <v>27416014289</v>
+      <c r="A11" s="1">
+        <v>45720974982</v>
+      </c>
+      <c r="B11" s="1">
+        <v>28012871460</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>45720974982</v>
-      </c>
-      <c r="B12" s="1">
-        <v>28012871460</v>
+      <c r="A12" s="2">
+        <v>44940297334</v>
+      </c>
+      <c r="B12" s="2">
+        <v>29686304354</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>44940297334</v>
-      </c>
-      <c r="B13" s="2">
-        <v>29686304354</v>
+      <c r="A13" s="1">
+        <v>47152285148</v>
+      </c>
+      <c r="B13" s="1">
+        <v>30583094069</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>47152285148</v>
-      </c>
-      <c r="B14" s="1">
-        <v>30583094069</v>
+      <c r="A14" s="2">
+        <v>45620914058</v>
+      </c>
+      <c r="B14" s="2">
+        <v>30650134267</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>45620914058</v>
-      </c>
-      <c r="B15" s="2">
-        <v>30650134267</v>
+      <c r="A15" s="1">
+        <v>47230510376</v>
+      </c>
+      <c r="B15" s="1">
+        <v>30348203314</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>47230510376</v>
-      </c>
-      <c r="B16" s="1">
-        <v>30348203314</v>
+      <c r="A16" s="2">
+        <v>47551517917</v>
+      </c>
+      <c r="B16" s="2">
+        <v>30214340879</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>47551517917</v>
-      </c>
-      <c r="B17" s="2">
-        <v>30214340879</v>
+      <c r="A17" s="1">
+        <v>48690050121</v>
+      </c>
+      <c r="B17" s="1">
+        <v>33575145734</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>48690050121</v>
-      </c>
-      <c r="B18" s="1">
-        <v>33575145734</v>
+      <c r="A18" s="2">
+        <v>47786091616</v>
+      </c>
+      <c r="B18" s="2">
+        <v>32422495953</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>47786091616</v>
-      </c>
-      <c r="B19" s="2">
-        <v>32422495953</v>
+      <c r="A19" s="1">
+        <v>47676902292</v>
+      </c>
+      <c r="B19" s="1">
+        <v>32054841279</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>47676902292</v>
-      </c>
-      <c r="B20" s="1">
-        <v>32054841279</v>
+      <c r="A20" s="2">
+        <v>46501390778</v>
+      </c>
+      <c r="B20" s="2">
+        <v>31690233060</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>46501390778</v>
-      </c>
-      <c r="B21" s="2">
-        <v>31690233060</v>
+      <c r="A21" s="1">
+        <v>47676992878</v>
+      </c>
+      <c r="B21" s="1">
+        <v>31540003049</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>47676992878</v>
-      </c>
-      <c r="B22" s="1">
-        <v>31540003049</v>
+      <c r="A22" s="2">
+        <v>48197217289</v>
+      </c>
+      <c r="B22" s="2">
+        <v>31735955230</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>48197217289</v>
-      </c>
-      <c r="B23" s="2">
-        <v>31735955230</v>
+      <c r="A23" s="1">
+        <v>47377636289</v>
+      </c>
+      <c r="B23" s="1">
+        <v>32590087552</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>47377636289</v>
-      </c>
-      <c r="B24" s="1">
-        <v>32590087552</v>
+      <c r="A24" s="2">
+        <v>46497545857</v>
+      </c>
+      <c r="B24" s="2">
+        <v>33324893690</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>46497545857</v>
-      </c>
-      <c r="B25" s="2">
-        <v>33324893690</v>
+      <c r="A25" s="3">
+        <f>AVERAGE(A2:A24)</f>
+        <v>44970354029.173912</v>
+      </c>
+      <c r="B25" s="3">
+        <f>AVERAGE(B2:B24)</f>
+        <v>27673057504.434784</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <f>_xlfn.STDEV.P(A2:A24)</f>
+        <v>4568806056.4124622</v>
+      </c>
+      <c r="B26" s="4">
+        <f>_xlfn.STDEV.P(B2:B24)</f>
+        <v>4996996196.6819315</v>
       </c>
     </row>
   </sheetData>
@@ -598,10 +633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319AC324-4248-4C3E-8841-E5B5EFCA5C5F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,83 +654,95 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>48014016657</v>
-      </c>
-      <c r="B2" s="1">
-        <v>42283885170</v>
+      <c r="A2" s="2">
+        <v>40318846789</v>
+      </c>
+      <c r="B2" s="2">
+        <v>36484584149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>40318846789</v>
-      </c>
-      <c r="B3" s="2">
-        <v>36484584149</v>
+      <c r="A3" s="1">
+        <v>40393003500</v>
+      </c>
+      <c r="B3" s="1">
+        <v>37305800173</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>40393003500</v>
-      </c>
-      <c r="B4" s="1">
-        <v>37305800173</v>
+      <c r="A4" s="2">
+        <v>39356104566</v>
+      </c>
+      <c r="B4" s="2">
+        <v>35770673462</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>39356104566</v>
-      </c>
-      <c r="B5" s="2">
-        <v>35770673462</v>
+      <c r="A5" s="1">
+        <v>44893925095</v>
+      </c>
+      <c r="B5" s="1">
+        <v>36907221291</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44893925095</v>
-      </c>
-      <c r="B6" s="1">
-        <v>36907221291</v>
+      <c r="A6" s="2">
+        <v>40158087630</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36791291940</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>40158087630</v>
-      </c>
-      <c r="B7" s="2">
-        <v>36791291940</v>
+      <c r="A7" s="1">
+        <v>40585858553</v>
+      </c>
+      <c r="B7" s="1">
+        <v>36252667897</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>40585858553</v>
-      </c>
-      <c r="B8" s="1">
-        <v>36252667897</v>
+      <c r="A8" s="2">
+        <v>40636752028</v>
+      </c>
+      <c r="B8" s="2">
+        <v>39026133623</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>40636752028</v>
-      </c>
-      <c r="B9" s="2">
-        <v>39026133623</v>
+      <c r="A9" s="1">
+        <v>40598330311</v>
+      </c>
+      <c r="B9" s="1">
+        <v>36988924271</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>40598330311</v>
-      </c>
-      <c r="B10" s="1">
-        <v>36988924271</v>
+      <c r="A10" s="2">
+        <v>40913688321</v>
+      </c>
+      <c r="B10" s="2">
+        <v>35451024956</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>40913688321</v>
-      </c>
-      <c r="B11" s="2">
-        <v>35451024956</v>
+      <c r="A11" s="3">
+        <f>AVERAGE(A2:A10)</f>
+        <v>40872732977</v>
+      </c>
+      <c r="B11" s="3">
+        <f>AVERAGE(B2:B10)</f>
+        <v>36775369084.666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f>_xlfn.STDEV.P(A2:A10)</f>
+        <v>1480718824.9110134</v>
+      </c>
+      <c r="B12" s="4">
+        <f>_xlfn.STDEV.P(B2:B10)</f>
+        <v>973630980.82922983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>